<commit_message>
se configura excel para persistir los datos de compra
</commit_message>
<xml_diff>
--- a/data/factura_ocr.xlsx
+++ b/data/factura_ocr.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,15 +479,11 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+      <c r="C2" t="n">
+        <v>44</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -514,15 +510,11 @@
       <c r="B3" t="n">
         <v>445922</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>45900</t>
-        </is>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>45900</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -549,15 +541,11 @@
       <c r="B4" t="n">
         <v>294588</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>57</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -584,15 +572,11 @@
       <c r="B5" t="n">
         <v>86320</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>47</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -613,21 +597,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Quesitto</t>
+          <t>Quesito</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="C6" t="n">
+        <v>21</v>
+      </c>
+      <c r="D6" t="n">
+        <v>21</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -654,15 +634,11 @@
       <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="C7" t="n">
+        <v>31</v>
+      </c>
+      <c r="D7" t="n">
+        <v>31</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -689,15 +665,11 @@
       <c r="B8" t="n">
         <v>1</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="C8" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" t="n">
+        <v>9</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,15 +696,11 @@
       <c r="B9" t="n">
         <v>1</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
+      <c r="C9" t="n">
+        <v>77</v>
+      </c>
+      <c r="D9" t="n">
+        <v>77</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -753,21 +721,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Miel</t>
+          <t>Mie!</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="C10" t="n">
+        <v>45</v>
+      </c>
+      <c r="D10" t="n">
+        <v>45</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -788,21 +752,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mantequi lla</t>
+          <t>Mantequilla</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
+      <c r="C11" t="n">
+        <v>51</v>
+      </c>
+      <c r="D11" t="n">
+        <v>51</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -829,15 +789,11 @@
       <c r="B12" t="n">
         <v>1</v>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
+      <c r="C12" t="n">
+        <v>52</v>
+      </c>
+      <c r="D12" t="n">
+        <v>52</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -864,15 +820,11 @@
       <c r="B13" t="n">
         <v>1</v>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>81000</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>81000</t>
-        </is>
+      <c r="C13" t="n">
+        <v>81000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>81000</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -885,6 +837,829 @@
         </is>
       </c>
       <c r="G13" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Hatsu</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>44</v>
+      </c>
+      <c r="D14" t="n">
+        <v>44</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>bebida sin alcohol</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>sp</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>445922</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>45900</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Pech</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>294588</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>57</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Cerdo</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>86320</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>47</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>carnes rojas</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Quesito</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>21</v>
+      </c>
+      <c r="D18" t="n">
+        <v>21</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>HuevosAA 60</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>31</v>
+      </c>
+      <c r="D19" t="n">
+        <v>31</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>carnes blancas</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Fideos</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>9</v>
+      </c>
+      <c r="D20" t="n">
+        <v>9</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>cereales</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Colageno</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>77</v>
+      </c>
+      <c r="D21" t="n">
+        <v>77</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Mie!</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>45</v>
+      </c>
+      <c r="D22" t="n">
+        <v>45</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Mantequilla</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>51</v>
+      </c>
+      <c r="D23" t="n">
+        <v>51</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>lácteos</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>AguaSaborix</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>52</v>
+      </c>
+      <c r="D24" t="n">
+        <v>52</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>bebida sin alcohol</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>cerveza</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>81000</v>
+      </c>
+      <c r="D25" t="n">
+        <v>81000</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>hamburguesa</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>15000</v>
+      </c>
+      <c r="D26" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>19/04/2025</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>por definir</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Hatsu</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>bebida sin alcohol</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>sp</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>445922</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>45900</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Pech</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>294588</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Cerdo</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>86320</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>carnes rojas</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Ques! to</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>HuevosAA 60</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>carnes blancas</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Fideos</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>cereales</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Colageno</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Mie!</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Mantequi lla</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>lácteos</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>AguaSaborix</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>bebida sin alcohol</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Pricesmart</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Ve cea</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>otros</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>desconocida</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>Pricesmart</t>
         </is>

</xml_diff>

<commit_message>
lectura de OCR, creacion de archivo excel, y actualizacion de archivo excel, penmdeinte confirguracion dede ruta del excel
</commit_message>
<xml_diff>
--- a/data/factura_ocr.xlsx
+++ b/data/factura_ocr.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,17 +473,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hatsu</t>
+          <t>954969 Hatsu</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>44</v>
+        <v>49900</v>
       </c>
       <c r="D2" t="n">
-        <v>44</v>
+        <v>49900</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -504,17 +504,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sp</t>
+          <t>Filete Pech</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>445922</v>
+        <v>294588</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>45900</v>
+        <v>57</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -535,21 +535,21 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pech</t>
+          <t>Lomo Cerdo</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>294588</v>
+        <v>86320</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>carnes rojas</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -566,21 +566,21 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cerdo</t>
+          <t>490035 Ques!to</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>86320</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D5" t="n">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>carnes rojas</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -597,21 +597,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Quesito</t>
+          <t>316919 HuevosAA 60</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D6" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>carnes blancas</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -628,21 +628,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HuevosAA 60</t>
+          <t>490538 Fideos</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>carnes blancas</t>
+          <t>cereales</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -659,21 +659,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Fideos</t>
+          <t>457997 Colageno</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D8" t="n">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>cereales</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -690,17 +690,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Colageno</t>
+          <t>455969 Miel</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="D9" t="n">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -721,21 +721,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mie!</t>
+          <t>357817 Mantequilla</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D10" t="n">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>lácteos</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -752,21 +752,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mantequilla</t>
+          <t>362118 AguaSabor1x</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>lácteos</t>
+          <t>bebida sin alcohol</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -783,21 +783,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AguaSaborix</t>
+          <t>27735 KSR6dCUPZ4D</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="D12" t="n">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>bebida sin alcohol</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -814,17 +814,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>cerveza</t>
+          <t>B— FEFL</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>81000</v>
+        <v>210</v>
       </c>
       <c r="D13" t="n">
-        <v>81000</v>
+        <v>1687</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -838,24 +838,28 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Pricesmart</t>
+          <t>por definir</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hatsu</t>
+          <t>954969 Hatsu</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
-      <c r="C14" t="n">
-        <v>44</v>
-      </c>
-      <c r="D14" t="n">
-        <v>44</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>49900</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>49900</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -876,17 +880,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>sp</t>
+          <t>Filete Pech</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>445922</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>45900</v>
+        <v>294588</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -907,21 +915,25 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Pech</t>
+          <t>Lomo Cerdo</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>294588</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>57</v>
+        <v>86320</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>carnes rojas</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -938,21 +950,25 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Cerdo</t>
+          <t>490035 Ques!to</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>86320</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>47</v>
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>carnes rojas</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -969,21 +985,25 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Quesito</t>
+          <t>316919 HuevosAA 60</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
-      <c r="C18" t="n">
-        <v>21</v>
-      </c>
-      <c r="D18" t="n">
-        <v>21</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>carnes blancas</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1000,21 +1020,25 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>HuevosAA 60</t>
+          <t>490538 Fideos</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>1</v>
       </c>
-      <c r="C19" t="n">
-        <v>31</v>
-      </c>
-      <c r="D19" t="n">
-        <v>31</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>carnes blancas</t>
+          <t>cereales</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1031,21 +1055,25 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Fideos</t>
+          <t>457997 Colageno</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>1</v>
       </c>
-      <c r="C20" t="n">
-        <v>9</v>
-      </c>
-      <c r="D20" t="n">
-        <v>9</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>cereales</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1062,17 +1090,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Colageno</t>
+          <t>455969 Miel</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>1</v>
       </c>
-      <c r="C21" t="n">
-        <v>77</v>
-      </c>
-      <c r="D21" t="n">
-        <v>77</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1093,21 +1125,25 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Mie!</t>
+          <t>357817 Mantequilla</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>1</v>
       </c>
-      <c r="C22" t="n">
-        <v>45</v>
-      </c>
-      <c r="D22" t="n">
-        <v>45</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>lácteos</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1124,21 +1160,25 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Mantequilla</t>
+          <t>362118 AguaSabor1x</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>1</v>
       </c>
-      <c r="C23" t="n">
-        <v>51</v>
-      </c>
-      <c r="D23" t="n">
-        <v>51</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>lácteos</t>
+          <t>bebida sin alcohol</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1155,21 +1195,25 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>AguaSaborix</t>
+          <t>27735 KSR6dCUPZ4D</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>1</v>
       </c>
-      <c r="C24" t="n">
-        <v>52</v>
-      </c>
-      <c r="D24" t="n">
-        <v>52</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>bebida sin alcohol</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1178,488 +1222,6 @@
         </is>
       </c>
       <c r="G24" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>cerveza</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" t="n">
-        <v>81000</v>
-      </c>
-      <c r="D25" t="n">
-        <v>81000</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>otros</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>hamburguesa</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" t="n">
-        <v>15000</v>
-      </c>
-      <c r="D26" t="n">
-        <v>15000</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>otros</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>19/04/2025</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>por definir</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Hatsu</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>bebida sin alcohol</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>sp</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>445922</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>45900</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>otros</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Pech</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>294588</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>otros</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Cerdo</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>86320</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>carnes rojas</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Ques! to</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>otros</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>HuevosAA 60</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>carnes blancas</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Fideos</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>cereales</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Colageno</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>otros</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Mie!</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>otros</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Mantequi lla</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>lácteos</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>AguaSaborix</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>bebida sin alcohol</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Ve cea</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>otros</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
         <is>
           <t>Pricesmart</t>
         </is>

</xml_diff>

<commit_message>
se añade la estructura de la factura10 y factura12
</commit_message>
<xml_diff>
--- a/data/factura_ocr.xlsx
+++ b/data/factura_ocr.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,52 +473,52 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>954969 Hatsu</t>
+          <t>Cappucu1no Pq 150 m1 1 8</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="C2" t="n">
-        <v>49900</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>49900</v>
+        <v>500</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>bebida sin alcohol</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>desconocida</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pricesmart</t>
+          <t>por definir</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Filete Pech</t>
+          <t>Hatsu</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>294588</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>49900</v>
       </c>
       <c r="D3" t="n">
-        <v>57</v>
+        <v>49900</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>bebida sin alcohol</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -535,21 +535,21 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lomo Cerdo</t>
+          <t>Filete Pech</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>86320</v>
+        <v>294588</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>carnes rojas</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -566,21 +566,21 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>490035 Ques!to</t>
+          <t>Lomo Cerdo</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>86320</v>
       </c>
       <c r="C5" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>carnes rojas</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -597,21 +597,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>316919 HuevosAA 60</t>
+          <t>Ques!to</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>carnes blancas</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -628,21 +628,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>490538 Fideos</t>
+          <t>HuevosAA 60</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D7" t="n">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>cereales</t>
+          <t>carnes blancas</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -659,21 +659,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>457997 Colageno</t>
+          <t>Fideos</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>cereales</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -690,17 +690,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>455969 Miel</t>
+          <t>Colageno</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="D9" t="n">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -721,21 +721,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>357817 Mantequilla</t>
+          <t>Miel</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D10" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>lácteos</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -752,7 +752,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>362118 AguaSabor1x</t>
+          <t>Mantequilla</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -766,7 +766,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>bebida sin alcohol</t>
+          <t>lácteos</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -783,21 +783,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>27735 KSR6dCUPZ4D</t>
+          <t>AguaSabor1x</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="D12" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>bebida sin alcohol</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -814,17 +814,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>B— FEFL</t>
+          <t>KSR6dCUPZ4D</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>210</v>
+        <v>82</v>
       </c>
       <c r="D13" t="n">
-        <v>1687</v>
+        <v>82</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -838,28 +838,24 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>por definir</t>
+          <t>Pricesmart</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>954969 Hatsu</t>
+          <t>Hatsu</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>49900</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>49900</t>
-        </is>
+      <c r="C14" t="n">
+        <v>49900</v>
+      </c>
+      <c r="D14" t="n">
+        <v>49900</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -886,19 +882,15 @@
       <c r="B15" t="n">
         <v>294588</v>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>58</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>otros</t>
+          <t>carnes blancas</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -921,15 +913,11 @@
       <c r="B16" t="n">
         <v>86320</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>48</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -950,21 +938,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>490035 Ques!to</t>
+          <t>Quesito</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>1</v>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="C17" t="n">
+        <v>22</v>
+      </c>
+      <c r="D17" t="n">
+        <v>22</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -985,25 +969,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>316919 HuevosAA 60</t>
+          <t>HuevosAA 60</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="C18" t="n">
+        <v>32</v>
+      </c>
+      <c r="D18" t="n">
+        <v>32</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>carnes blancas</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1020,25 +1000,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>490538 Fideos</t>
+          <t>Fideos</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>1</v>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="C19" t="n">
+        <v>10</v>
+      </c>
+      <c r="D19" t="n">
+        <v>10</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>cereales</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1055,21 +1031,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>457997 Colageno</t>
+          <t>i 333342 Almendra21b</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>1</v>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
+      <c r="C20" t="n">
+        <v>46</v>
+      </c>
+      <c r="D20" t="n">
+        <v>46</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1090,21 +1062,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>455969 Miel</t>
+          <t>cerveza</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>1</v>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="C21" t="n">
+        <v>82000</v>
+      </c>
+      <c r="D21" t="n">
+        <v>82000</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1125,7 +1093,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>357817 Mantequilla</t>
+          <t>Cappucu1no Pq 150 m1 1 8 500 8</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1133,97 +1101,27 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>500</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>500</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>lácteos</t>
+          <t>otros</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>desconocida</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>362118 AguaSabor1x</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>bebida sin alcohol</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>27735 KSR6dCUPZ4D</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>otros</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>desconocida</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Pricesmart</t>
+          <t>por definir</t>
         </is>
       </c>
     </row>

</xml_diff>